<commit_message>
Added support for am domain (in _ccm.py), now doesn't load all components and all configs unless needed
If you specify a GC then all components and configs not loaded - saves a lot of time on very large projects with many components and configs
If you specify a GC _and_ and local component and a local config then the config URL is found using the GC contribution and the query is made to that local config - avoids having to load all the configs in the component!
If you specify a component and a local config then only the configs for that component are loaded
AM support added but NOTE it doesn't currently (7.0.2) have any useful OSLC query capability even though there is a QueryCapability there aren't any shapes - not clear if this will change
</commit_message>
<xml_diff>
--- a/elmclient/tests/tests_702.xlsx
+++ b/elmclient/tests/tests_702.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{520E8122-7CDD-44B8-9C85-39633DBC5707}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C08D47E-0D53-4D4A-BD2E-A18E336EEDA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1183" yWindow="857" windowWidth="22834" windowHeight="14597" xr2:uid="{E12FDD20-F1C7-4695-B929-60D3CA2A8B69}"/>
+    <workbookView xWindow="32550" yWindow="-18600" windowWidth="22830" windowHeight="14595" xr2:uid="{E12FDD20-F1C7-4695-B929-60D3CA2A8B69}"/>
   </bookViews>
   <sheets>
     <sheet name="rmqueries" sheetId="1" r:id="rId1"/>
@@ -576,9 +576,6 @@
     <t>SGC AMR</t>
   </si>
   <si>
-    <t>ETM app qiuery configurations across all project</t>
-  </si>
-  <si>
     <t>ETM app query components across all project</t>
   </si>
   <si>
@@ -715,6 +712,9 @@
   </si>
   <si>
     <t># FAILS!</t>
+  </si>
+  <si>
+    <t>ETM app query configurations across all projects</t>
   </si>
 </sst>
 </file>
@@ -1164,8 +1164,8 @@
   <dimension ref="A1:AH110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F39" sqref="F39"/>
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A91" sqref="A91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1328,7 +1328,7 @@
     </row>
     <row r="3" spans="1:34" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A3" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
@@ -1433,7 +1433,7 @@
     </row>
     <row r="6" spans="1:34" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A6" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>82</v>
@@ -1757,7 +1757,7 @@
         <v>106</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C14" s="5">
         <f t="shared" si="3"/>
@@ -1773,7 +1773,7 @@
         <v>105</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="K14" s="7"/>
       <c r="L14" s="7"/>
@@ -1805,7 +1805,7 @@
         <v>106</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C15" s="5">
         <f t="shared" si="3"/>
@@ -1853,7 +1853,7 @@
         <v>106</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C16" s="5">
         <f t="shared" si="3"/>
@@ -1898,7 +1898,7 @@
     </row>
     <row r="17" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A17" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>82</v>
@@ -2716,7 +2716,7 @@
         <v>133</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F36" s="5">
         <v>1478</v>
@@ -2766,7 +2766,7 @@
         <v>739</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I37" s="8"/>
       <c r="M37" s="6" t="str">
@@ -2777,7 +2777,7 @@
         <v>114</v>
       </c>
       <c r="R37" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="S37" s="5" t="s">
         <v>114</v>
@@ -2810,7 +2810,7 @@
         <v>739</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I38" s="8"/>
       <c r="M38" s="6" t="str">
@@ -2821,10 +2821,10 @@
         <v>114</v>
       </c>
       <c r="R38" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="S38" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="V38" s="5" t="s">
         <v>12</v>
@@ -2854,7 +2854,7 @@
         <v>51</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I39" s="8"/>
       <c r="K39" s="5" t="s">
@@ -2904,7 +2904,7 @@
         <v>8</v>
       </c>
       <c r="L40" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="M40" s="6" t="str">
         <f t="shared" si="0"/>
@@ -2986,7 +2986,7 @@
         <v>128</v>
       </c>
       <c r="H42" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I42" s="8"/>
       <c r="L42" s="6"/>
@@ -3064,7 +3064,7 @@
         <v>141</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F44" s="5">
         <v>1652</v>
@@ -3078,13 +3078,13 @@
         <v>tests\results\test141.csv</v>
       </c>
       <c r="Q44" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="T44" s="5" t="s">
         <v>89</v>
       </c>
       <c r="U44" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="V44" s="5" t="s">
         <v>12</v>
@@ -3114,7 +3114,7 @@
         <v>325</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I45" s="8"/>
       <c r="M45" s="6" t="str">
@@ -3122,13 +3122,13 @@
         <v>tests\results\test142.csv</v>
       </c>
       <c r="Q45" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="R45" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="S45" s="5" t="s">
         <v>197</v>
-      </c>
-      <c r="R45" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="S45" s="5" t="s">
-        <v>198</v>
       </c>
       <c r="V45" s="5" t="s">
         <v>12</v>
@@ -3158,7 +3158,7 @@
         <v>744</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I46" s="8"/>
       <c r="M46" s="6" t="str">
@@ -3166,10 +3166,10 @@
         <v>tests\results\test143.csv</v>
       </c>
       <c r="Q46" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="R46" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="S46" s="5" t="s">
         <v>181</v>
@@ -3202,7 +3202,7 @@
         <v>583</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I47" s="8"/>
       <c r="M47" s="6" t="str">
@@ -3210,7 +3210,7 @@
         <v>tests\results\test144.csv</v>
       </c>
       <c r="Q47" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="R47" s="5" t="s">
         <v>81</v>
@@ -3231,10 +3231,10 @@
         <v>92</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I48" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J48" s="5" t="s">
         <v>8</v>
@@ -3275,10 +3275,10 @@
         <v>62</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I49" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J49" s="5" t="s">
         <v>8</v>
@@ -3319,10 +3319,10 @@
         <v>92</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I50" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="J50" s="5" t="s">
         <v>8</v>
@@ -3363,10 +3363,10 @@
         <v>0</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I51" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J51" s="5" t="s">
         <v>8</v>
@@ -3407,10 +3407,10 @@
         <v>92</v>
       </c>
       <c r="G52" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="I52" s="5" t="s">
         <v>222</v>
-      </c>
-      <c r="I52" s="5" t="s">
-        <v>223</v>
       </c>
       <c r="J52" s="5" t="s">
         <v>8</v>
@@ -3441,7 +3441,7 @@
     </row>
     <row r="53" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A53" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>82</v>
@@ -3454,7 +3454,7 @@
         <v>0</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I53" s="9" t="s">
         <v>170</v>
@@ -3489,7 +3489,7 @@
     <row r="54" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.4"/>
     <row r="56" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A56" s="9" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="57" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.4">
@@ -3506,7 +3506,7 @@
         <v>16</v>
       </c>
       <c r="G57" s="9" t="s">
-        <v>182</v>
+        <v>228</v>
       </c>
       <c r="J57" s="9" t="s">
         <v>8</v>
@@ -3543,10 +3543,10 @@
         <v>9</v>
       </c>
       <c r="G58" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I58" s="9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="M58" s="13" t="str">
         <f t="shared" si="15"/>
@@ -3580,7 +3580,7 @@
         <v>4</v>
       </c>
       <c r="G59" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H59" s="9" t="s">
         <v>35</v>
@@ -3883,7 +3883,7 @@
     <row r="67" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.4"/>
     <row r="69" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A69" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="70" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.4">
@@ -4032,7 +4032,7 @@
         <v>162</v>
       </c>
       <c r="I73" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J73" s="4" t="s">
         <v>8</v>
@@ -4330,10 +4330,10 @@
         <v>2</v>
       </c>
       <c r="G80" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I80" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="M80" s="11" t="str">
         <f t="shared" si="25"/>
@@ -4370,7 +4370,7 @@
         <v>0</v>
       </c>
       <c r="G81" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J81" s="4" t="s">
         <v>8</v>
@@ -4380,7 +4380,7 @@
         <v>tests\results\test312.csv</v>
       </c>
       <c r="N81" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="Q81" s="4" t="s">
         <v>87</v>
@@ -4535,7 +4535,7 @@
         <v>5</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H90" s="3" t="s">
         <v>35</v>
@@ -4575,7 +4575,7 @@
         <v>4</v>
       </c>
       <c r="G91" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H91" s="3" t="s">
         <v>35</v>
@@ -4621,7 +4621,7 @@
         <v>24</v>
       </c>
       <c r="G92" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H92" s="3" t="s">
         <v>36</v>
@@ -4670,7 +4670,7 @@
         <v>1</v>
       </c>
       <c r="G93" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H93" s="3" t="s">
         <v>35</v>
@@ -4706,7 +4706,7 @@
     <row r="96" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.4"/>
     <row r="98" spans="1:31" s="14" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A98" s="14" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G98" s="14" t="s">
         <v>153</v>

</xml_diff>

<commit_message>
minor version update - ran oslcquery tests against 7.0.2SR1
</commit_message>
<xml_diff>
--- a/elmclient/tests/tests_702.xlsx
+++ b/elmclient/tests/tests_702.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C08D47E-0D53-4D4A-BD2E-A18E336EEDA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5606ACDF-AA38-42D5-A112-05261FB8CF9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32550" yWindow="-18600" windowWidth="22830" windowHeight="14595" xr2:uid="{E12FDD20-F1C7-4695-B929-60D3CA2A8B69}"/>
+    <workbookView xWindow="1183" yWindow="2237" windowWidth="24686" windowHeight="13106" xr2:uid="{E12FDD20-F1C7-4695-B929-60D3CA2A8B69}"/>
   </bookViews>
   <sheets>
     <sheet name="rmqueries" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="232">
   <si>
     <t>oslc_rm:uses</t>
   </si>
@@ -708,13 +708,22 @@
     <t>rm,gc</t>
   </si>
   <si>
-    <t>All artifacts created by fred</t>
-  </si>
-  <si>
-    <t># FAILS!</t>
-  </si>
-  <si>
     <t>ETM app query configurations across all projects</t>
+  </si>
+  <si>
+    <t>All modules of type 'Stakeholder Specification'</t>
+  </si>
+  <si>
+    <t>All artifacts created by tanuj</t>
+  </si>
+  <si>
+    <t># doesn't work</t>
+  </si>
+  <si>
+    <t>App query for just streams and baselines</t>
+  </si>
+  <si>
+    <t>rdf:type in [oslc_config:Baseline, oslc_config:Stream]</t>
   </si>
 </sst>
 </file>
@@ -1161,11 +1170,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34CC5532-4E98-4C99-BC3C-1388DFEBC8F1}">
-  <dimension ref="A1:AH110"/>
+  <dimension ref="A1:AH111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A91" sqref="A91"/>
+      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F95" sqref="F95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1439,7 +1448,7 @@
         <v>82</v>
       </c>
       <c r="C6" s="5">
-        <f t="shared" ref="C6:C53" si="3">C5+1</f>
+        <f t="shared" ref="C6:C54" si="3">C5+1</f>
         <v>103</v>
       </c>
       <c r="G6" s="5" t="s">
@@ -3251,7 +3260,7 @@
         <v>12</v>
       </c>
       <c r="W48" s="5" t="str">
-        <f t="shared" ref="W48:X53" si="8">W$2</f>
+        <f t="shared" ref="W48:X54" si="8">W$2</f>
         <v>ibm</v>
       </c>
       <c r="X48" s="5" t="str">
@@ -3259,7 +3268,7 @@
         <v>ibm</v>
       </c>
       <c r="Y48" s="5" t="str">
-        <f t="shared" ref="Y48:Y53" si="9">Y$2</f>
+        <f t="shared" ref="Y48:Y54" si="9">Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -3441,7 +3450,7 @@
     </row>
     <row r="53" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A53" s="5" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>82</v>
@@ -3454,7 +3463,7 @@
         <v>0</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="I53" s="9" t="s">
         <v>170</v>
@@ -3486,46 +3495,54 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="54" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="56" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A56" s="9" t="s">
+    <row r="54" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B54" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C54" s="5">
+        <f t="shared" si="3"/>
+        <v>151</v>
+      </c>
+      <c r="F54" s="5">
+        <v>1</v>
+      </c>
+      <c r="G54" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="I54" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="J54" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="L54" s="6"/>
+      <c r="M54" s="6" t="str">
+        <f t="shared" ref="M54" si="15">"tests\results\test"&amp;C54&amp;".csv"</f>
+        <v>tests\results\test151.csv</v>
+      </c>
+      <c r="Q54" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="V54" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="W54" s="5" t="str">
+        <f t="shared" si="8"/>
+        <v>ibm</v>
+      </c>
+      <c r="X54" s="5" t="str">
+        <f t="shared" si="8"/>
+        <v>ibm</v>
+      </c>
+      <c r="Y54" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>https://jazz.ibm.com:9443</v>
+      </c>
+    </row>
+    <row r="55" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="57" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A57" s="9" t="s">
         <v>207</v>
-      </c>
-    </row>
-    <row r="57" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="B57" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="C57" s="9">
-        <v>201</v>
-      </c>
-      <c r="E57" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="F57" s="9">
-        <v>16</v>
-      </c>
-      <c r="G57" s="9" t="s">
-        <v>228</v>
-      </c>
-      <c r="J57" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="M57" s="13" t="str">
-        <f t="shared" ref="M57:M58" si="15">"tests\results\test"&amp;C57&amp;".csv"</f>
-        <v>tests\results\test201.csv</v>
-      </c>
-      <c r="W57" s="9" t="str">
-        <f t="shared" ref="W57:X66" si="16">W$2</f>
-        <v>ibm</v>
-      </c>
-      <c r="X57" s="9" t="str">
-        <f t="shared" si="16"/>
-        <v>ibm</v>
-      </c>
-      <c r="Y57" s="9" t="str">
-        <f t="shared" ref="Y57:Y66" si="17">Y$2</f>
-        <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="58" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.4">
@@ -3533,35 +3550,34 @@
         <v>83</v>
       </c>
       <c r="C58" s="9">
-        <f>C57+1</f>
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E58" s="9" t="s">
         <v>72</v>
       </c>
       <c r="F58" s="9">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="G58" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="I58" s="9" t="s">
-        <v>211</v>
+        <v>226</v>
+      </c>
+      <c r="J58" s="9" t="s">
+        <v>8</v>
       </c>
       <c r="M58" s="13" t="str">
-        <f t="shared" si="15"/>
-        <v>tests\results\test202.csv</v>
+        <f t="shared" ref="M58:M59" si="16">"tests\results\test"&amp;C58&amp;".csv"</f>
+        <v>tests\results\test201.csv</v>
       </c>
       <c r="W58" s="9" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" ref="W58:X67" si="17">W$2</f>
         <v>ibm</v>
       </c>
       <c r="X58" s="9" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>ibm</v>
       </c>
       <c r="Y58" s="9" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" ref="Y58:Y67" si="18">Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -3570,35 +3586,35 @@
         <v>83</v>
       </c>
       <c r="C59" s="9">
-        <f t="shared" ref="C59:C64" si="18">C58+1</f>
-        <v>203</v>
+        <f>C58+1</f>
+        <v>202</v>
       </c>
       <c r="E59" s="9" t="s">
         <v>72</v>
       </c>
       <c r="F59" s="9">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="G59" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="H59" s="9" t="s">
-        <v>35</v>
+        <v>223</v>
+      </c>
+      <c r="I59" s="9" t="s">
+        <v>211</v>
       </c>
       <c r="M59" s="13" t="str">
-        <f t="shared" ref="M59" si="19">"tests\results\test"&amp;C59&amp;".csv"</f>
-        <v>tests\results\test203.csv</v>
+        <f t="shared" si="16"/>
+        <v>tests\results\test202.csv</v>
       </c>
       <c r="W59" s="9" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>ibm</v>
       </c>
       <c r="X59" s="9" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>ibm</v>
       </c>
       <c r="Y59" s="9" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -3607,70 +3623,58 @@
         <v>83</v>
       </c>
       <c r="C60" s="9">
-        <f t="shared" si="18"/>
-        <v>204</v>
+        <f t="shared" ref="C60:C65" si="19">C59+1</f>
+        <v>203</v>
       </c>
       <c r="E60" s="9" t="s">
         <v>72</v>
       </c>
       <c r="F60" s="9">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="G60" s="9" t="s">
-        <v>95</v>
+        <v>182</v>
+      </c>
+      <c r="H60" s="9" t="s">
+        <v>35</v>
       </c>
       <c r="M60" s="13" t="str">
-        <f t="shared" ref="M60:M61" si="20">"tests\results\test"&amp;C60&amp;".csv"</f>
-        <v>tests\results\test204.csv</v>
-      </c>
-      <c r="Q60" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="R60" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="S60" s="9" t="s">
-        <v>79</v>
+        <f t="shared" ref="M60" si="20">"tests\results\test"&amp;C60&amp;".csv"</f>
+        <v>tests\results\test203.csv</v>
       </c>
       <c r="W60" s="9" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>ibm</v>
       </c>
       <c r="X60" s="9" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>ibm</v>
       </c>
       <c r="Y60" s="9" t="str">
-        <f t="shared" si="17"/>
-        <v>https://jazz.ibm.com:9443</v>
-      </c>
-      <c r="AA60" s="9" t="s">
-        <v>125</v>
+        <f t="shared" si="18"/>
+        <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="61" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B61" s="9" t="s">
-        <v>169</v>
+        <v>83</v>
       </c>
       <c r="C61" s="9">
-        <f t="shared" si="18"/>
-        <v>205</v>
+        <f t="shared" si="19"/>
+        <v>204</v>
       </c>
       <c r="E61" s="9" t="s">
         <v>72</v>
       </c>
       <c r="F61" s="9">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="G61" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="H61" s="9" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="M61" s="13" t="str">
-        <f t="shared" si="20"/>
-        <v>tests\results\test205.csv</v>
+        <f t="shared" ref="M61:M62" si="21">"tests\results\test"&amp;C61&amp;".csv"</f>
+        <v>tests\results\test204.csv</v>
       </c>
       <c r="Q61" s="9" t="s">
         <v>78</v>
@@ -3682,16 +3686,19 @@
         <v>79</v>
       </c>
       <c r="W61" s="9" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>ibm</v>
       </c>
       <c r="X61" s="9" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>ibm</v>
       </c>
       <c r="Y61" s="9" t="str">
-        <f t="shared" si="17"/>
-        <v>https://jazz.ibm.com:9443</v>
+        <f t="shared" si="18"/>
+        <v>https://jazz.ibm.com:9443</v>
+      </c>
+      <c r="AA61" s="9" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="62" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.4">
@@ -3699,23 +3706,23 @@
         <v>169</v>
       </c>
       <c r="C62" s="9">
-        <f t="shared" si="18"/>
-        <v>206</v>
+        <f t="shared" si="19"/>
+        <v>205</v>
       </c>
       <c r="E62" s="9" t="s">
         <v>72</v>
       </c>
       <c r="F62" s="9">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="G62" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="I62" s="9" t="s">
-        <v>170</v>
+        <v>96</v>
+      </c>
+      <c r="H62" s="9" t="s">
+        <v>92</v>
       </c>
       <c r="M62" s="13" t="str">
-        <f>"tests\results\test"&amp;C61&amp;".csv"</f>
+        <f t="shared" si="21"/>
         <v>tests\results\test205.csv</v>
       </c>
       <c r="Q62" s="9" t="s">
@@ -3728,15 +3735,15 @@
         <v>79</v>
       </c>
       <c r="W62" s="9" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>ibm</v>
       </c>
       <c r="X62" s="9" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>ibm</v>
       </c>
       <c r="Y62" s="9" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -3745,24 +3752,24 @@
         <v>169</v>
       </c>
       <c r="C63" s="9">
-        <f t="shared" si="18"/>
-        <v>207</v>
+        <f t="shared" si="19"/>
+        <v>206</v>
       </c>
       <c r="E63" s="9" t="s">
         <v>72</v>
       </c>
       <c r="F63" s="9">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="G63" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
+      </c>
+      <c r="I63" s="9" t="s">
+        <v>170</v>
       </c>
       <c r="M63" s="13" t="str">
         <f>"tests\results\test"&amp;C62&amp;".csv"</f>
-        <v>tests\results\test206.csv</v>
-      </c>
-      <c r="N63" s="9" t="s">
-        <v>173</v>
+        <v>tests\results\test205.csv</v>
       </c>
       <c r="Q63" s="9" t="s">
         <v>78</v>
@@ -3774,15 +3781,15 @@
         <v>79</v>
       </c>
       <c r="W63" s="9" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>ibm</v>
       </c>
       <c r="X63" s="9" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>ibm</v>
       </c>
       <c r="Y63" s="9" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -3791,23 +3798,23 @@
         <v>169</v>
       </c>
       <c r="C64" s="9">
-        <f t="shared" si="18"/>
-        <v>208</v>
+        <f t="shared" si="19"/>
+        <v>207</v>
       </c>
       <c r="E64" s="9" t="s">
         <v>72</v>
       </c>
       <c r="F64" s="9">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="G64" s="9" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="M64" s="13" t="str">
         <f>"tests\results\test"&amp;C63&amp;".csv"</f>
-        <v>tests\results\test207.csv</v>
-      </c>
-      <c r="P64" s="9" t="s">
+        <v>tests\results\test206.csv</v>
+      </c>
+      <c r="N64" s="9" t="s">
         <v>173</v>
       </c>
       <c r="Q64" s="9" t="s">
@@ -3820,20 +3827,42 @@
         <v>79</v>
       </c>
       <c r="W64" s="9" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>ibm</v>
       </c>
       <c r="X64" s="9" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>ibm</v>
       </c>
       <c r="Y64" s="9" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="65" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="M65" s="13"/>
+      <c r="B65" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="C65" s="9">
+        <f t="shared" si="19"/>
+        <v>208</v>
+      </c>
+      <c r="E65" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="F65" s="9">
+        <v>8</v>
+      </c>
+      <c r="G65" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="M65" s="13" t="str">
+        <f>"tests\results\test"&amp;C64&amp;".csv"</f>
+        <v>tests\results\test207.csv</v>
+      </c>
+      <c r="P65" s="9" t="s">
+        <v>173</v>
+      </c>
       <c r="Q65" s="9" t="s">
         <v>78</v>
       </c>
@@ -3844,15 +3873,15 @@
         <v>79</v>
       </c>
       <c r="W65" s="9" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>ibm</v>
       </c>
       <c r="X65" s="9" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>ibm</v>
       </c>
       <c r="Y65" s="9" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -3868,107 +3897,88 @@
         <v>79</v>
       </c>
       <c r="W66" s="9" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>ibm</v>
       </c>
       <c r="X66" s="9" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>ibm</v>
       </c>
       <c r="Y66" s="9" t="str">
+        <f t="shared" si="18"/>
+        <v>https://jazz.ibm.com:9443</v>
+      </c>
+    </row>
+    <row r="67" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="M67" s="13"/>
+      <c r="Q67" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="R67" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="S67" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="W67" s="9" t="str">
         <f t="shared" si="17"/>
-        <v>https://jazz.ibm.com:9443</v>
-      </c>
-    </row>
-    <row r="67" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="69" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A69" s="4" t="s">
+        <v>ibm</v>
+      </c>
+      <c r="X67" s="9" t="str">
+        <f t="shared" si="17"/>
+        <v>ibm</v>
+      </c>
+      <c r="Y67" s="9" t="str">
+        <f t="shared" si="18"/>
+        <v>https://jazz.ibm.com:9443</v>
+      </c>
+    </row>
+    <row r="68" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="70" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A70" s="4" t="s">
         <v>209</v>
-      </c>
-    </row>
-    <row r="70" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="B70" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C70" s="4">
-        <v>301</v>
-      </c>
-      <c r="E70" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="F70" s="4">
-        <v>89</v>
-      </c>
-      <c r="G70" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="J70" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="M70" s="11" t="str">
-        <f t="shared" ref="M70:M76" si="21">"tests\results\test"&amp;C70&amp;".csv"</f>
-        <v>tests\results\test301.csv</v>
-      </c>
-      <c r="Q70" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="W70" s="4" t="str">
-        <f t="shared" ref="W70:X85" si="22">W$2</f>
-        <v>ibm</v>
-      </c>
-      <c r="X70" s="4" t="str">
-        <f t="shared" si="22"/>
-        <v>ibm</v>
-      </c>
-      <c r="Y70" s="4" t="str">
-        <f t="shared" ref="Y70:Y85" si="23">Y$2</f>
-        <v>https://jazz.ibm.com:9443</v>
-      </c>
-      <c r="AA70" s="4" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="71" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B71" s="4" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="C71" s="4">
-        <f>C70+1</f>
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E71" s="4" t="s">
         <v>73</v>
       </c>
       <c r="F71" s="4">
-        <v>34</v>
+        <v>89</v>
       </c>
       <c r="G71" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="I71" s="11" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="J71" s="4" t="s">
         <v>8</v>
       </c>
       <c r="M71" s="11" t="str">
-        <f t="shared" si="21"/>
-        <v>tests\results\test302.csv</v>
+        <f t="shared" ref="M71:M77" si="22">"tests\results\test"&amp;C71&amp;".csv"</f>
+        <v>tests\results\test301.csv</v>
       </c>
       <c r="Q71" s="4" t="s">
         <v>87</v>
       </c>
       <c r="W71" s="4" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" ref="W71:X86" si="23">W$2</f>
         <v>ibm</v>
       </c>
       <c r="X71" s="4" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>ibm</v>
       </c>
       <c r="Y71" s="4" t="str">
-        <f t="shared" si="23"/>
-        <v>https://jazz.ibm.com:9443</v>
+        <f t="shared" ref="Y71:Y86" si="24">Y$2</f>
+        <v>https://jazz.ibm.com:9443</v>
+      </c>
+      <c r="AA71" s="4" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="72" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.4">
@@ -3976,41 +3986,41 @@
         <v>98</v>
       </c>
       <c r="C72" s="4">
-        <f t="shared" ref="C72:C81" si="24">C71+1</f>
-        <v>303</v>
+        <f>C71+1</f>
+        <v>302</v>
       </c>
       <c r="E72" s="4" t="s">
         <v>73</v>
       </c>
       <c r="F72" s="4">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="G72" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="I72" s="4" t="s">
-        <v>160</v>
+        <v>99</v>
+      </c>
+      <c r="I72" s="11" t="s">
+        <v>100</v>
       </c>
       <c r="J72" s="4" t="s">
         <v>8</v>
       </c>
       <c r="M72" s="11" t="str">
-        <f t="shared" si="21"/>
-        <v>tests\results\test303.csv</v>
+        <f t="shared" si="22"/>
+        <v>tests\results\test302.csv</v>
       </c>
       <c r="Q72" s="4" t="s">
         <v>87</v>
       </c>
       <c r="W72" s="4" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>ibm</v>
       </c>
       <c r="X72" s="4" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>ibm</v>
       </c>
       <c r="Y72" s="4" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -4019,41 +4029,41 @@
         <v>98</v>
       </c>
       <c r="C73" s="4">
-        <f t="shared" si="24"/>
-        <v>304</v>
+        <f t="shared" ref="C73:C82" si="25">C72+1</f>
+        <v>303</v>
       </c>
       <c r="E73" s="4" t="s">
         <v>73</v>
       </c>
       <c r="F73" s="4">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="G73" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I73" s="4" t="s">
-        <v>206</v>
+        <v>160</v>
       </c>
       <c r="J73" s="4" t="s">
         <v>8</v>
       </c>
       <c r="M73" s="11" t="str">
-        <f t="shared" si="21"/>
-        <v>tests\results\test304.csv</v>
+        <f t="shared" si="22"/>
+        <v>tests\results\test303.csv</v>
       </c>
       <c r="Q73" s="4" t="s">
         <v>87</v>
       </c>
       <c r="W73" s="4" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>ibm</v>
       </c>
       <c r="X73" s="4" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>ibm</v>
       </c>
       <c r="Y73" s="4" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -4062,41 +4072,41 @@
         <v>98</v>
       </c>
       <c r="C74" s="4">
-        <f t="shared" si="24"/>
-        <v>305</v>
+        <f t="shared" si="25"/>
+        <v>304</v>
       </c>
       <c r="E74" s="4" t="s">
         <v>73</v>
       </c>
       <c r="F74" s="4">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="G74" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
+      </c>
+      <c r="I74" s="4" t="s">
+        <v>206</v>
       </c>
       <c r="J74" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="K74" s="4" t="s">
-        <v>163</v>
-      </c>
       <c r="M74" s="11" t="str">
-        <f t="shared" si="21"/>
-        <v>tests\results\test305.csv</v>
+        <f t="shared" si="22"/>
+        <v>tests\results\test304.csv</v>
       </c>
       <c r="Q74" s="4" t="s">
         <v>87</v>
       </c>
       <c r="W74" s="4" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>ibm</v>
       </c>
       <c r="X74" s="4" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>ibm</v>
       </c>
       <c r="Y74" s="4" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -4105,41 +4115,41 @@
         <v>98</v>
       </c>
       <c r="C75" s="4">
-        <f t="shared" si="24"/>
-        <v>306</v>
+        <f t="shared" si="25"/>
+        <v>305</v>
       </c>
       <c r="E75" s="4" t="s">
         <v>73</v>
       </c>
       <c r="F75" s="4">
-        <v>89</v>
+        <v>12</v>
       </c>
       <c r="G75" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="I75" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J75" s="4" t="s">
         <v>8</v>
       </c>
+      <c r="K75" s="4" t="s">
+        <v>163</v>
+      </c>
       <c r="M75" s="11" t="str">
-        <f t="shared" si="21"/>
-        <v>tests\results\test306.csv</v>
+        <f t="shared" si="22"/>
+        <v>tests\results\test305.csv</v>
       </c>
       <c r="Q75" s="4" t="s">
         <v>87</v>
       </c>
       <c r="W75" s="4" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>ibm</v>
       </c>
       <c r="X75" s="4" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>ibm</v>
       </c>
       <c r="Y75" s="4" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -4148,41 +4158,41 @@
         <v>98</v>
       </c>
       <c r="C76" s="4">
-        <f t="shared" si="24"/>
-        <v>307</v>
+        <f t="shared" si="25"/>
+        <v>306</v>
       </c>
       <c r="E76" s="4" t="s">
         <v>73</v>
       </c>
       <c r="F76" s="4">
-        <v>0</v>
+        <v>89</v>
       </c>
       <c r="G76" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I76" s="4" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="J76" s="4" t="s">
         <v>8</v>
       </c>
       <c r="M76" s="11" t="str">
-        <f t="shared" si="21"/>
-        <v>tests\results\test307.csv</v>
+        <f t="shared" si="22"/>
+        <v>tests\results\test306.csv</v>
       </c>
       <c r="Q76" s="4" t="s">
         <v>87</v>
       </c>
       <c r="W76" s="4" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>ibm</v>
       </c>
       <c r="X76" s="4" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>ibm</v>
       </c>
       <c r="Y76" s="4" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -4191,41 +4201,41 @@
         <v>98</v>
       </c>
       <c r="C77" s="4">
-        <f t="shared" si="24"/>
-        <v>308</v>
+        <f t="shared" si="25"/>
+        <v>307</v>
       </c>
       <c r="E77" s="4" t="s">
         <v>73</v>
       </c>
       <c r="F77" s="4">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="G77" s="4" t="s">
-        <v>176</v>
+        <v>167</v>
+      </c>
+      <c r="I77" s="4" t="s">
+        <v>168</v>
       </c>
       <c r="J77" s="4" t="s">
         <v>8</v>
       </c>
       <c r="M77" s="11" t="str">
-        <f t="shared" ref="M77:M81" si="25">"tests\results\test"&amp;C77&amp;".csv"</f>
-        <v>tests\results\test308.csv</v>
-      </c>
-      <c r="N77" s="4" t="s">
-        <v>175</v>
+        <f t="shared" si="22"/>
+        <v>tests\results\test307.csv</v>
       </c>
       <c r="Q77" s="4" t="s">
         <v>87</v>
       </c>
       <c r="W77" s="4" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>ibm</v>
       </c>
       <c r="X77" s="4" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>ibm</v>
       </c>
       <c r="Y77" s="4" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -4234,41 +4244,41 @@
         <v>98</v>
       </c>
       <c r="C78" s="4">
-        <f t="shared" si="24"/>
-        <v>309</v>
+        <f t="shared" si="25"/>
+        <v>308</v>
       </c>
       <c r="E78" s="4" t="s">
         <v>73</v>
       </c>
       <c r="F78" s="4">
-        <v>66</v>
+        <v>23</v>
       </c>
       <c r="G78" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J78" s="4" t="s">
         <v>8</v>
       </c>
       <c r="M78" s="11" t="str">
-        <f t="shared" si="25"/>
-        <v>tests\results\test309.csv</v>
-      </c>
-      <c r="P78" s="4" t="s">
+        <f t="shared" ref="M78:M82" si="26">"tests\results\test"&amp;C78&amp;".csv"</f>
+        <v>tests\results\test308.csv</v>
+      </c>
+      <c r="N78" s="4" t="s">
         <v>175</v>
       </c>
       <c r="Q78" s="4" t="s">
         <v>87</v>
       </c>
       <c r="W78" s="4" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>ibm</v>
       </c>
       <c r="X78" s="4" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>ibm</v>
       </c>
       <c r="Y78" s="4" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -4277,41 +4287,41 @@
         <v>98</v>
       </c>
       <c r="C79" s="4">
-        <f t="shared" si="24"/>
-        <v>310</v>
+        <f t="shared" si="25"/>
+        <v>309</v>
       </c>
       <c r="E79" s="4" t="s">
         <v>73</v>
       </c>
       <c r="F79" s="4">
-        <v>38</v>
+        <v>66</v>
       </c>
       <c r="G79" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="I79" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J79" s="4" t="s">
         <v>8</v>
       </c>
       <c r="M79" s="11" t="str">
-        <f t="shared" si="25"/>
-        <v>tests\results\test310.csv</v>
+        <f t="shared" si="26"/>
+        <v>tests\results\test309.csv</v>
+      </c>
+      <c r="P79" s="4" t="s">
+        <v>175</v>
       </c>
       <c r="Q79" s="4" t="s">
         <v>87</v>
       </c>
       <c r="W79" s="4" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>ibm</v>
       </c>
       <c r="X79" s="4" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>ibm</v>
       </c>
       <c r="Y79" s="4" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -4320,38 +4330,41 @@
         <v>98</v>
       </c>
       <c r="C80" s="4">
-        <f t="shared" si="24"/>
-        <v>311</v>
+        <f t="shared" si="25"/>
+        <v>310</v>
       </c>
       <c r="E80" s="4" t="s">
         <v>73</v>
       </c>
       <c r="F80" s="4">
-        <v>2</v>
+        <v>38</v>
       </c>
       <c r="G80" s="4" t="s">
-        <v>205</v>
+        <v>179</v>
       </c>
       <c r="I80" s="4" t="s">
-        <v>204</v>
+        <v>178</v>
+      </c>
+      <c r="J80" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="M80" s="11" t="str">
-        <f t="shared" si="25"/>
-        <v>tests\results\test311.csv</v>
+        <f t="shared" si="26"/>
+        <v>tests\results\test310.csv</v>
       </c>
       <c r="Q80" s="4" t="s">
         <v>87</v>
       </c>
       <c r="W80" s="4" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>ibm</v>
       </c>
       <c r="X80" s="4" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>ibm</v>
       </c>
       <c r="Y80" s="4" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -4360,63 +4373,85 @@
         <v>98</v>
       </c>
       <c r="C81" s="4">
-        <f t="shared" si="24"/>
-        <v>312</v>
+        <f t="shared" si="25"/>
+        <v>311</v>
       </c>
       <c r="E81" s="4" t="s">
         <v>73</v>
       </c>
       <c r="F81" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G81" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="J81" s="4" t="s">
-        <v>8</v>
+        <v>205</v>
+      </c>
+      <c r="I81" s="4" t="s">
+        <v>204</v>
       </c>
       <c r="M81" s="11" t="str">
-        <f t="shared" si="25"/>
-        <v>tests\results\test312.csv</v>
-      </c>
-      <c r="N81" s="4" t="s">
-        <v>190</v>
+        <f t="shared" si="26"/>
+        <v>tests\results\test311.csv</v>
       </c>
       <c r="Q81" s="4" t="s">
         <v>87</v>
       </c>
       <c r="W81" s="4" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>ibm</v>
       </c>
       <c r="X81" s="4" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>ibm</v>
       </c>
       <c r="Y81" s="4" t="str">
-        <f t="shared" si="23"/>
-        <v>https://jazz.ibm.com:9443</v>
-      </c>
-      <c r="AA81" s="4" t="s">
-        <v>126</v>
+        <f t="shared" si="24"/>
+        <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="82" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="M82" s="11"/>
+      <c r="B82" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C82" s="4">
+        <f t="shared" si="25"/>
+        <v>312</v>
+      </c>
+      <c r="E82" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F82" s="4">
+        <v>0</v>
+      </c>
+      <c r="G82" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="J82" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M82" s="11" t="str">
+        <f t="shared" si="26"/>
+        <v>tests\results\test312.csv</v>
+      </c>
+      <c r="N82" s="4" t="s">
+        <v>190</v>
+      </c>
       <c r="Q82" s="4" t="s">
         <v>87</v>
       </c>
       <c r="W82" s="4" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>ibm</v>
       </c>
       <c r="X82" s="4" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>ibm</v>
       </c>
       <c r="Y82" s="4" t="str">
-        <f t="shared" si="23"/>
-        <v>https://jazz.ibm.com:9443</v>
+        <f t="shared" si="24"/>
+        <v>https://jazz.ibm.com:9443</v>
+      </c>
+      <c r="AA82" s="4" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="83" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.4">
@@ -4425,15 +4460,15 @@
         <v>87</v>
       </c>
       <c r="W83" s="4" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>ibm</v>
       </c>
       <c r="X83" s="4" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>ibm</v>
       </c>
       <c r="Y83" s="4" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -4443,15 +4478,15 @@
         <v>87</v>
       </c>
       <c r="W84" s="4" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>ibm</v>
       </c>
       <c r="X84" s="4" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>ibm</v>
       </c>
       <c r="Y84" s="4" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -4461,63 +4496,42 @@
         <v>87</v>
       </c>
       <c r="W85" s="4" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>ibm</v>
       </c>
       <c r="X85" s="4" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>ibm</v>
       </c>
       <c r="Y85" s="4" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="86" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="M86" s="11"/>
-    </row>
-    <row r="88" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A88" s="3" t="s">
+      <c r="Q86" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="W86" s="4" t="str">
+        <f t="shared" si="23"/>
+        <v>ibm</v>
+      </c>
+      <c r="X86" s="4" t="str">
+        <f t="shared" si="23"/>
+        <v>ibm</v>
+      </c>
+      <c r="Y86" s="4" t="str">
+        <f t="shared" si="24"/>
+        <v>https://jazz.ibm.com:9443</v>
+      </c>
+    </row>
+    <row r="87" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="M87" s="11"/>
+    </row>
+    <row r="89" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A89" s="3" t="s">
         <v>91</v>
-      </c>
-    </row>
-    <row r="89" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="B89" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C89" s="3">
-        <v>401</v>
-      </c>
-      <c r="E89" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="F89" s="3">
-        <v>26</v>
-      </c>
-      <c r="G89" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="H89" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="J89" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="M89" s="10" t="str">
-        <f t="shared" ref="M89:M93" si="26">"tests\results\test"&amp;C89&amp;".csv"</f>
-        <v>tests\results\test401.csv</v>
-      </c>
-      <c r="W89" s="3" t="str">
-        <f t="shared" ref="W89:X93" si="27">W$2</f>
-        <v>ibm</v>
-      </c>
-      <c r="X89" s="3" t="str">
-        <f t="shared" si="27"/>
-        <v>ibm</v>
-      </c>
-      <c r="Y89" s="3" t="str">
-        <f>Y$2</f>
-        <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="90" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.4">
@@ -4525,34 +4539,33 @@
         <v>85</v>
       </c>
       <c r="C90" s="3">
-        <f>C89+1</f>
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="E90" s="3" t="s">
         <v>77</v>
       </c>
       <c r="F90" s="3">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="H90" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J90" s="3" t="s">
         <v>8</v>
       </c>
       <c r="M90" s="10" t="str">
-        <f t="shared" ref="M90" si="28">"tests\results\test"&amp;C90&amp;".csv"</f>
-        <v>tests\results\test402.csv</v>
+        <f t="shared" ref="M90:M94" si="27">"tests\results\test"&amp;C90&amp;".csv"</f>
+        <v>tests\results\test401.csv</v>
       </c>
       <c r="W90" s="3" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" ref="W90:X95" si="28">W$2</f>
         <v>ibm</v>
       </c>
       <c r="X90" s="3" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>ibm</v>
       </c>
       <c r="Y90" s="3" t="str">
@@ -4565,17 +4578,17 @@
         <v>85</v>
       </c>
       <c r="C91" s="3">
-        <f t="shared" ref="C91:C93" si="29">C90+1</f>
-        <v>403</v>
+        <f>C90+1</f>
+        <v>402</v>
       </c>
       <c r="E91" s="3" t="s">
         <v>77</v>
       </c>
       <c r="F91" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G91" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H91" s="3" t="s">
         <v>35</v>
@@ -4584,26 +4597,20 @@
         <v>8</v>
       </c>
       <c r="M91" s="10" t="str">
-        <f t="shared" ref="M91" si="30">"tests\results\test"&amp;C91&amp;".csv"</f>
-        <v>tests\results\test403.csv</v>
-      </c>
-      <c r="Q91" s="3" t="s">
-        <v>89</v>
+        <f t="shared" ref="M91" si="29">"tests\results\test"&amp;C91&amp;".csv"</f>
+        <v>tests\results\test402.csv</v>
       </c>
       <c r="W91" s="3" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>ibm</v>
       </c>
       <c r="X91" s="3" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>ibm</v>
       </c>
       <c r="Y91" s="3" t="str">
         <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
-      </c>
-      <c r="AA91" s="3" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="92" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.4">
@@ -4611,89 +4618,89 @@
         <v>85</v>
       </c>
       <c r="C92" s="3">
-        <f t="shared" si="29"/>
-        <v>404</v>
+        <f t="shared" ref="C92:C95" si="30">C91+1</f>
+        <v>403</v>
       </c>
       <c r="E92" s="3" t="s">
         <v>77</v>
       </c>
       <c r="F92" s="3">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="G92" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H92" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J92" s="3" t="s">
         <v>8</v>
       </c>
       <c r="M92" s="10" t="str">
-        <f t="shared" si="26"/>
-        <v>tests\results\test404.csv</v>
+        <f t="shared" ref="M92" si="31">"tests\results\test"&amp;C92&amp;".csv"</f>
+        <v>tests\results\test403.csv</v>
       </c>
       <c r="Q92" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="R92" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="S92" s="3" t="s">
-        <v>181</v>
-      </c>
       <c r="W92" s="3" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>ibm</v>
       </c>
       <c r="X92" s="3" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>ibm</v>
       </c>
       <c r="Y92" s="3" t="str">
         <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
+      <c r="AA92" s="3" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="93" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B93" s="3" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="C93" s="3">
-        <f t="shared" si="29"/>
-        <v>405</v>
+        <f t="shared" si="30"/>
+        <v>404</v>
       </c>
       <c r="E93" s="3" t="s">
         <v>77</v>
       </c>
       <c r="F93" s="3">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="G93" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H93" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="I93" s="10" t="s">
-        <v>108</v>
+        <v>36</v>
       </c>
       <c r="J93" s="3" t="s">
         <v>8</v>
       </c>
       <c r="M93" s="10" t="str">
-        <f t="shared" si="26"/>
-        <v>tests\results\test405.csv</v>
+        <f t="shared" si="27"/>
+        <v>tests\results\test404.csv</v>
       </c>
       <c r="Q93" s="3" t="s">
         <v>89</v>
       </c>
+      <c r="R93" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="S93" s="3" t="s">
+        <v>181</v>
+      </c>
       <c r="W93" s="3" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>ibm</v>
       </c>
       <c r="X93" s="3" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>ibm</v>
       </c>
       <c r="Y93" s="3" t="str">
@@ -4701,35 +4708,109 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="94" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="95" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="94" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="B94" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C94" s="3">
+        <f t="shared" si="30"/>
+        <v>405</v>
+      </c>
+      <c r="E94" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F94" s="3">
+        <v>1</v>
+      </c>
+      <c r="G94" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="H94" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I94" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="J94" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M94" s="10" t="str">
+        <f t="shared" si="27"/>
+        <v>tests\results\test405.csv</v>
+      </c>
+      <c r="Q94" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="W94" s="3" t="str">
+        <f t="shared" si="28"/>
+        <v>ibm</v>
+      </c>
+      <c r="X94" s="3" t="str">
+        <f t="shared" si="28"/>
+        <v>ibm</v>
+      </c>
+      <c r="Y94" s="3" t="str">
+        <f>Y$2</f>
+        <v>https://jazz.ibm.com:9443</v>
+      </c>
+    </row>
+    <row r="95" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="B95" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C95" s="3">
+        <f t="shared" si="30"/>
+        <v>406</v>
+      </c>
+      <c r="E95" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F95" s="3">
+        <v>24</v>
+      </c>
+      <c r="G95" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="H95" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I95" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="J95" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M95" s="10" t="str">
+        <f t="shared" ref="M95" si="32">"tests\results\test"&amp;C95&amp;".csv"</f>
+        <v>tests\results\test406.csv</v>
+      </c>
+      <c r="Q95" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="S95" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="W95" s="3" t="str">
+        <f t="shared" si="28"/>
+        <v>ibm</v>
+      </c>
+      <c r="X95" s="3" t="str">
+        <f t="shared" si="28"/>
+        <v>ibm</v>
+      </c>
+      <c r="Y95" s="3" t="str">
+        <f>Y$2</f>
+        <v>https://jazz.ibm.com:9443</v>
+      </c>
+    </row>
     <row r="96" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="98" spans="1:31" s="14" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A98" s="14" t="s">
+    <row r="97" spans="1:31" s="3" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="99" spans="1:31" s="14" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A99" s="14" t="s">
         <v>210</v>
       </c>
-      <c r="G98" s="14" t="s">
+      <c r="G99" s="14" t="s">
         <v>153</v>
-      </c>
-      <c r="I98" s="15"/>
-      <c r="J98" s="15"/>
-      <c r="K98" s="15"/>
-      <c r="L98" s="15"/>
-      <c r="M98" s="15"/>
-      <c r="N98" s="15"/>
-      <c r="O98" s="15"/>
-      <c r="P98" s="15"/>
-      <c r="Y98" s="16"/>
-    </row>
-    <row r="99" spans="1:31" s="14" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="B99" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="C99" s="14">
-        <v>1001</v>
-      </c>
-      <c r="G99" s="14" t="s">
-        <v>155</v>
       </c>
       <c r="I99" s="15"/>
       <c r="J99" s="15"/>
@@ -4739,46 +4820,17 @@
       <c r="N99" s="15"/>
       <c r="O99" s="15"/>
       <c r="P99" s="15"/>
-      <c r="Q99" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="R99" s="14" t="str">
-        <f t="shared" ref="R99:R108" si="31">Q99&amp;" Initial Stream"</f>
-        <v>rm_optout_p1 Initial Stream</v>
-      </c>
-      <c r="S99" s="14" t="str">
-        <f t="shared" ref="S99:S107" si="32">Q99</f>
-        <v>rm_optout_p1</v>
-      </c>
-      <c r="W99" s="5" t="str">
-        <f>W$2</f>
-        <v>ibm</v>
-      </c>
-      <c r="X99" s="5" t="str">
-        <f>X$2</f>
-        <v>ibm</v>
-      </c>
-      <c r="Y99" s="5" t="str">
-        <f>Y$2</f>
-        <v>https://jazz.ibm.com:9443</v>
-      </c>
-      <c r="AB99" s="14" t="s">
-        <v>142</v>
-      </c>
+      <c r="Y99" s="16"/>
     </row>
     <row r="100" spans="1:31" s="14" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B100" s="14" t="s">
         <v>141</v>
       </c>
       <c r="C100" s="14">
-        <f>C99+1</f>
-        <v>1002</v>
-      </c>
-      <c r="F100" s="14">
-        <v>738</v>
+        <v>1001</v>
       </c>
       <c r="G100" s="14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I100" s="15"/>
       <c r="J100" s="15"/>
@@ -4792,23 +4844,26 @@
         <v>11</v>
       </c>
       <c r="R100" s="14" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" ref="R100:R109" si="33">Q100&amp;" Initial Stream"</f>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S100" s="14" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" ref="S100:S108" si="34">Q100</f>
         <v>rm_optout_p1</v>
       </c>
-      <c r="W100" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="X100" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="Y100" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="AC100" s="14" t="s">
+      <c r="W100" s="5" t="str">
+        <f>W$2</f>
+        <v>ibm</v>
+      </c>
+      <c r="X100" s="5" t="str">
+        <f>X$2</f>
+        <v>ibm</v>
+      </c>
+      <c r="Y100" s="5" t="str">
+        <f>Y$2</f>
+        <v>https://jazz.ibm.com:9443</v>
+      </c>
+      <c r="AB100" s="14" t="s">
         <v>142</v>
       </c>
     </row>
@@ -4817,14 +4872,14 @@
         <v>141</v>
       </c>
       <c r="C101" s="14">
-        <f t="shared" ref="C101:C108" si="33">C100+1</f>
-        <v>1003</v>
-      </c>
-      <c r="D101" s="14" t="s">
-        <v>143</v>
+        <f>C100+1</f>
+        <v>1002</v>
+      </c>
+      <c r="F101" s="14">
+        <v>738</v>
       </c>
       <c r="G101" s="14" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="I101" s="15"/>
       <c r="J101" s="15"/>
@@ -4838,11 +4893,11 @@
         <v>11</v>
       </c>
       <c r="R101" s="14" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S101" s="14" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>rm_optout_p1</v>
       </c>
       <c r="W101" s="14" t="s">
@@ -4856,9 +4911,6 @@
       </c>
       <c r="AC101" s="14" t="s">
         <v>142</v>
-      </c>
-      <c r="AE101" s="14" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="102" spans="1:31" s="14" customFormat="1" x14ac:dyDescent="0.4">
@@ -4866,11 +4918,14 @@
         <v>141</v>
       </c>
       <c r="C102" s="14">
-        <f t="shared" si="33"/>
-        <v>1004</v>
+        <f t="shared" ref="C102:C109" si="35">C101+1</f>
+        <v>1003</v>
+      </c>
+      <c r="D102" s="14" t="s">
+        <v>143</v>
       </c>
       <c r="G102" s="14" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="I102" s="15"/>
       <c r="J102" s="15"/>
@@ -4884,11 +4939,11 @@
         <v>11</v>
       </c>
       <c r="R102" s="14" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S102" s="14" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>rm_optout_p1</v>
       </c>
       <c r="W102" s="14" t="s">
@@ -4900,8 +4955,11 @@
       <c r="Y102" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="AD102" s="14" t="s">
+      <c r="AC102" s="14" t="s">
         <v>142</v>
+      </c>
+      <c r="AE102" s="14" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="103" spans="1:31" s="14" customFormat="1" x14ac:dyDescent="0.4">
@@ -4909,14 +4967,11 @@
         <v>141</v>
       </c>
       <c r="C103" s="14">
-        <f t="shared" si="33"/>
-        <v>1005</v>
-      </c>
-      <c r="D103" s="14" t="s">
-        <v>143</v>
+        <f t="shared" si="35"/>
+        <v>1004</v>
       </c>
       <c r="G103" s="14" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="I103" s="15"/>
       <c r="J103" s="15"/>
@@ -4930,11 +4985,11 @@
         <v>11</v>
       </c>
       <c r="R103" s="14" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S103" s="14" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>rm_optout_p1</v>
       </c>
       <c r="W103" s="14" t="s">
@@ -4946,7 +5001,7 @@
       <c r="Y103" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="AC103" s="14" t="s">
+      <c r="AD103" s="14" t="s">
         <v>142</v>
       </c>
     </row>
@@ -4955,11 +5010,14 @@
         <v>141</v>
       </c>
       <c r="C104" s="14">
-        <f t="shared" si="33"/>
-        <v>1006</v>
+        <f t="shared" si="35"/>
+        <v>1005</v>
+      </c>
+      <c r="D104" s="14" t="s">
+        <v>143</v>
       </c>
       <c r="G104" s="14" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="I104" s="15"/>
       <c r="J104" s="15"/>
@@ -4973,30 +5031,24 @@
         <v>11</v>
       </c>
       <c r="R104" s="14" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S104" s="14" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>rm_optout_p1</v>
       </c>
-      <c r="W104" s="5" t="str">
-        <f>W$2</f>
-        <v>ibm</v>
-      </c>
-      <c r="X104" s="5" t="str">
-        <f>X$2</f>
-        <v>ibm</v>
-      </c>
-      <c r="Y104" s="5" t="str">
-        <f>Y$2</f>
-        <v>https://jazz.ibm.com:9443</v>
-      </c>
-      <c r="AB104" s="14" t="s">
+      <c r="W104" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="X104" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="Y104" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="AC104" s="14" t="s">
         <v>142</v>
-      </c>
-      <c r="AE104" s="14" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="105" spans="1:31" s="14" customFormat="1" x14ac:dyDescent="0.4">
@@ -5004,11 +5056,11 @@
         <v>141</v>
       </c>
       <c r="C105" s="14">
-        <f t="shared" si="33"/>
-        <v>1007</v>
+        <f t="shared" si="35"/>
+        <v>1006</v>
       </c>
       <c r="G105" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I105" s="15"/>
       <c r="J105" s="15"/>
@@ -5022,23 +5074,26 @@
         <v>11</v>
       </c>
       <c r="R105" s="14" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S105" s="14" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>rm_optout_p1</v>
       </c>
-      <c r="W105" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="X105" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="Y105" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="AC105" s="14" t="s">
+      <c r="W105" s="5" t="str">
+        <f>W$2</f>
+        <v>ibm</v>
+      </c>
+      <c r="X105" s="5" t="str">
+        <f>X$2</f>
+        <v>ibm</v>
+      </c>
+      <c r="Y105" s="5" t="str">
+        <f>Y$2</f>
+        <v>https://jazz.ibm.com:9443</v>
+      </c>
+      <c r="AB105" s="14" t="s">
         <v>142</v>
       </c>
       <c r="AE105" s="14" t="s">
@@ -5050,14 +5105,11 @@
         <v>141</v>
       </c>
       <c r="C106" s="14">
-        <f t="shared" si="33"/>
-        <v>1008</v>
-      </c>
-      <c r="D106" s="14" t="s">
-        <v>143</v>
+        <f t="shared" si="35"/>
+        <v>1007</v>
       </c>
       <c r="G106" s="14" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="I106" s="15"/>
       <c r="J106" s="15"/>
@@ -5071,11 +5123,11 @@
         <v>11</v>
       </c>
       <c r="R106" s="14" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S106" s="14" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>rm_optout_p1</v>
       </c>
       <c r="W106" s="14" t="s">
@@ -5091,7 +5143,7 @@
         <v>142</v>
       </c>
       <c r="AE106" s="14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="107" spans="1:31" s="14" customFormat="1" x14ac:dyDescent="0.4">
@@ -5099,14 +5151,14 @@
         <v>141</v>
       </c>
       <c r="C107" s="14">
-        <f t="shared" si="33"/>
-        <v>1009</v>
+        <f t="shared" si="35"/>
+        <v>1008</v>
       </c>
       <c r="D107" s="14" t="s">
         <v>143</v>
       </c>
       <c r="G107" s="14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I107" s="15"/>
       <c r="J107" s="15"/>
@@ -5120,11 +5172,11 @@
         <v>11</v>
       </c>
       <c r="R107" s="14" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S107" s="14" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>rm_optout_p1</v>
       </c>
       <c r="W107" s="14" t="s">
@@ -5138,6 +5190,9 @@
       </c>
       <c r="AC107" s="14" t="s">
         <v>142</v>
+      </c>
+      <c r="AE107" s="14" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="108" spans="1:31" s="14" customFormat="1" x14ac:dyDescent="0.4">
@@ -5145,11 +5200,14 @@
         <v>141</v>
       </c>
       <c r="C108" s="14">
-        <f t="shared" si="33"/>
-        <v>1010</v>
+        <f t="shared" si="35"/>
+        <v>1009</v>
+      </c>
+      <c r="D108" s="14" t="s">
+        <v>143</v>
       </c>
       <c r="G108" s="14" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="I108" s="15"/>
       <c r="J108" s="15"/>
@@ -5163,11 +5221,11 @@
         <v>11</v>
       </c>
       <c r="R108" s="14" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S108" s="14" t="str">
-        <f t="shared" ref="S108" si="34">Q108</f>
+        <f t="shared" si="34"/>
         <v>rm_optout_p1</v>
       </c>
       <c r="W108" s="14" t="s">
@@ -5179,11 +5237,21 @@
       <c r="Y108" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="AD108" s="14" t="s">
+      <c r="AC108" s="14" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="109" spans="1:31" s="14" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="B109" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="C109" s="14">
+        <f t="shared" si="35"/>
+        <v>1010</v>
+      </c>
+      <c r="G109" s="14" t="s">
+        <v>144</v>
+      </c>
       <c r="I109" s="15"/>
       <c r="J109" s="15"/>
       <c r="K109" s="15"/>
@@ -5192,18 +5260,51 @@
       <c r="N109" s="15"/>
       <c r="O109" s="15"/>
       <c r="P109" s="15"/>
-      <c r="Y109" s="16"/>
-    </row>
-    <row r="110" spans="1:31" x14ac:dyDescent="0.4">
-      <c r="I110" s="2"/>
-      <c r="J110" s="2"/>
-      <c r="K110" s="2"/>
-      <c r="L110" s="2"/>
-      <c r="M110" s="2"/>
-      <c r="N110" s="2"/>
-      <c r="O110" s="2"/>
-      <c r="P110" s="2"/>
-      <c r="Y110" s="12"/>
+      <c r="Q109" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="R109" s="14" t="str">
+        <f t="shared" si="33"/>
+        <v>rm_optout_p1 Initial Stream</v>
+      </c>
+      <c r="S109" s="14" t="str">
+        <f t="shared" ref="S109" si="36">Q109</f>
+        <v>rm_optout_p1</v>
+      </c>
+      <c r="W109" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="X109" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="Y109" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="AD109" s="14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="110" spans="1:31" s="14" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="I110" s="15"/>
+      <c r="J110" s="15"/>
+      <c r="K110" s="15"/>
+      <c r="L110" s="15"/>
+      <c r="M110" s="15"/>
+      <c r="N110" s="15"/>
+      <c r="O110" s="15"/>
+      <c r="P110" s="15"/>
+      <c r="Y110" s="16"/>
+    </row>
+    <row r="111" spans="1:31" x14ac:dyDescent="0.4">
+      <c r="I111" s="2"/>
+      <c r="J111" s="2"/>
+      <c r="K111" s="2"/>
+      <c r="L111" s="2"/>
+      <c r="M111" s="2"/>
+      <c r="N111" s="2"/>
+      <c r="O111" s="2"/>
+      <c r="P111" s="2"/>
+      <c r="Y111" s="12"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
oslcquery: fixed problem with link columns not being checked correctly for -v/-n
</commit_message>
<xml_diff>
--- a/elmclient/tests/tests_702.xlsx
+++ b/elmclient/tests/tests_702.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5606ACDF-AA38-42D5-A112-05261FB8CF9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B073099B-4FDA-4E28-869F-2EDAC9172B2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1183" yWindow="2237" windowWidth="24686" windowHeight="13106" xr2:uid="{E12FDD20-F1C7-4695-B929-60D3CA2A8B69}"/>
+    <workbookView xWindow="1414" yWindow="4080" windowWidth="24686" windowHeight="13054" xr2:uid="{E12FDD20-F1C7-4695-B929-60D3CA2A8B69}"/>
   </bookViews>
   <sheets>
     <sheet name="rmqueries" sheetId="1" r:id="rId1"/>
@@ -669,9 +669,6 @@
     <t>-dcterms:modified</t>
   </si>
   <si>
-    <t>rm:module=~3892</t>
-  </si>
-  <si>
     <t>All artifacts in module 3892 of artifact type Stakehilder Requirement</t>
   </si>
   <si>
@@ -681,15 +678,6 @@
     <t>All artifacts in module 3892 modified before a date</t>
   </si>
   <si>
-    <t>rm:module=~3892 and oslc:instanceShape='Stakeholder Requirement'</t>
-  </si>
-  <si>
-    <t>rm:module=~3892 and dcterms:modified&lt;"2012-08-01T21:51:40.979Z"^^xsd:dateTime</t>
-  </si>
-  <si>
-    <t>rm:module=~3892 and dcterms:modified&gt;"2012-08-01T21:51:40.979Z"^^xsd:dateTime</t>
-  </si>
-  <si>
     <t>All artifacts in module 3892 Stakeholder Requirements</t>
   </si>
   <si>
@@ -724,6 +712,18 @@
   </si>
   <si>
     <t>rdf:type in [oslc_config:Baseline, oslc_config:Stream]</t>
+  </si>
+  <si>
+    <t>rm:module=~3891</t>
+  </si>
+  <si>
+    <t>rm:module=~3891 and oslc:instanceShape='Stakeholder Requirement'</t>
+  </si>
+  <si>
+    <t>rm:module=~3891 and dcterms:modified&gt;"2012-08-01T21:51:40.979Z"^^xsd:dateTime</t>
+  </si>
+  <si>
+    <t>rm:module=~3891 and dcterms:modified&lt;"2012-08-01T21:51:40.979Z"^^xsd:dateTime</t>
   </si>
 </sst>
 </file>
@@ -1172,9 +1172,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34CC5532-4E98-4C99-BC3C-1388DFEBC8F1}">
   <dimension ref="A1:AH111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F95" sqref="F95"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F82" sqref="F82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1442,7 +1442,7 @@
     </row>
     <row r="6" spans="1:34" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A6" s="5" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>82</v>
@@ -1907,7 +1907,7 @@
     </row>
     <row r="17" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A17" s="5" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>82</v>
@@ -2725,7 +2725,7 @@
         <v>133</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="F36" s="5">
         <v>1478</v>
@@ -3073,7 +3073,7 @@
         <v>141</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="F44" s="5">
         <v>1652</v>
@@ -3240,10 +3240,10 @@
         <v>92</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="I48" s="5" t="s">
-        <v>213</v>
+        <v>228</v>
       </c>
       <c r="J48" s="5" t="s">
         <v>8</v>
@@ -3284,10 +3284,10 @@
         <v>62</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I49" s="5" t="s">
-        <v>217</v>
+        <v>229</v>
       </c>
       <c r="J49" s="5" t="s">
         <v>8</v>
@@ -3328,10 +3328,10 @@
         <v>92</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I50" s="5" t="s">
-        <v>219</v>
+        <v>230</v>
       </c>
       <c r="J50" s="5" t="s">
         <v>8</v>
@@ -3372,10 +3372,10 @@
         <v>0</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I51" s="5" t="s">
-        <v>218</v>
+        <v>231</v>
       </c>
       <c r="J51" s="5" t="s">
         <v>8</v>
@@ -3416,10 +3416,10 @@
         <v>92</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="I52" s="5" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="J52" s="5" t="s">
         <v>8</v>
@@ -3450,7 +3450,7 @@
     </row>
     <row r="53" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A53" s="5" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>82</v>
@@ -3463,7 +3463,7 @@
         <v>0</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="I53" s="9" t="s">
         <v>170</v>
@@ -3507,7 +3507,7 @@
         <v>1</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="I54" s="8" t="s">
         <v>45</v>
@@ -3559,7 +3559,7 @@
         <v>16</v>
       </c>
       <c r="G58" s="9" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="J58" s="9" t="s">
         <v>8</v>
@@ -3596,7 +3596,7 @@
         <v>9</v>
       </c>
       <c r="G59" s="9" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="I59" s="9" t="s">
         <v>211</v>
@@ -4380,7 +4380,7 @@
         <v>73</v>
       </c>
       <c r="F81" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G81" s="4" t="s">
         <v>205</v>
@@ -4569,7 +4569,7 @@
         <v>ibm</v>
       </c>
       <c r="Y90" s="3" t="str">
-        <f>Y$2</f>
+        <f t="shared" ref="Y90:Y95" si="29">Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -4597,7 +4597,7 @@
         <v>8</v>
       </c>
       <c r="M91" s="10" t="str">
-        <f t="shared" ref="M91" si="29">"tests\results\test"&amp;C91&amp;".csv"</f>
+        <f t="shared" ref="M91" si="30">"tests\results\test"&amp;C91&amp;".csv"</f>
         <v>tests\results\test402.csv</v>
       </c>
       <c r="W91" s="3" t="str">
@@ -4609,7 +4609,7 @@
         <v>ibm</v>
       </c>
       <c r="Y91" s="3" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="29"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -4618,7 +4618,7 @@
         <v>85</v>
       </c>
       <c r="C92" s="3">
-        <f t="shared" ref="C92:C95" si="30">C91+1</f>
+        <f t="shared" ref="C92:C95" si="31">C91+1</f>
         <v>403</v>
       </c>
       <c r="E92" s="3" t="s">
@@ -4637,7 +4637,7 @@
         <v>8</v>
       </c>
       <c r="M92" s="10" t="str">
-        <f t="shared" ref="M92" si="31">"tests\results\test"&amp;C92&amp;".csv"</f>
+        <f t="shared" ref="M92" si="32">"tests\results\test"&amp;C92&amp;".csv"</f>
         <v>tests\results\test403.csv</v>
       </c>
       <c r="Q92" s="3" t="s">
@@ -4652,7 +4652,7 @@
         <v>ibm</v>
       </c>
       <c r="Y92" s="3" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="29"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
       <c r="AA92" s="3" t="s">
@@ -4664,7 +4664,7 @@
         <v>85</v>
       </c>
       <c r="C93" s="3">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>404</v>
       </c>
       <c r="E93" s="3" t="s">
@@ -4704,7 +4704,7 @@
         <v>ibm</v>
       </c>
       <c r="Y93" s="3" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="29"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -4713,7 +4713,7 @@
         <v>97</v>
       </c>
       <c r="C94" s="3">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>405</v>
       </c>
       <c r="E94" s="3" t="s">
@@ -4750,7 +4750,7 @@
         <v>ibm</v>
       </c>
       <c r="Y94" s="3" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="29"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -4759,7 +4759,7 @@
         <v>97</v>
       </c>
       <c r="C95" s="3">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>406</v>
       </c>
       <c r="E95" s="3" t="s">
@@ -4769,19 +4769,19 @@
         <v>24</v>
       </c>
       <c r="G95" s="3" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="H95" s="3" t="s">
         <v>36</v>
       </c>
       <c r="I95" s="3" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="J95" s="3" t="s">
         <v>8</v>
       </c>
       <c r="M95" s="10" t="str">
-        <f t="shared" ref="M95" si="32">"tests\results\test"&amp;C95&amp;".csv"</f>
+        <f t="shared" ref="M95" si="33">"tests\results\test"&amp;C95&amp;".csv"</f>
         <v>tests\results\test406.csv</v>
       </c>
       <c r="Q95" s="3" t="s">
@@ -4799,7 +4799,7 @@
         <v>ibm</v>
       </c>
       <c r="Y95" s="3" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="29"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -4844,11 +4844,11 @@
         <v>11</v>
       </c>
       <c r="R100" s="14" t="str">
-        <f t="shared" ref="R100:R109" si="33">Q100&amp;" Initial Stream"</f>
+        <f t="shared" ref="R100:R109" si="34">Q100&amp;" Initial Stream"</f>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S100" s="14" t="str">
-        <f t="shared" ref="S100:S108" si="34">Q100</f>
+        <f t="shared" ref="S100:S108" si="35">Q100</f>
         <v>rm_optout_p1</v>
       </c>
       <c r="W100" s="5" t="str">
@@ -4893,11 +4893,11 @@
         <v>11</v>
       </c>
       <c r="R101" s="14" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S101" s="14" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>rm_optout_p1</v>
       </c>
       <c r="W101" s="14" t="s">
@@ -4918,7 +4918,7 @@
         <v>141</v>
       </c>
       <c r="C102" s="14">
-        <f t="shared" ref="C102:C109" si="35">C101+1</f>
+        <f t="shared" ref="C102:C109" si="36">C101+1</f>
         <v>1003</v>
       </c>
       <c r="D102" s="14" t="s">
@@ -4939,11 +4939,11 @@
         <v>11</v>
       </c>
       <c r="R102" s="14" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S102" s="14" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>rm_optout_p1</v>
       </c>
       <c r="W102" s="14" t="s">
@@ -4967,7 +4967,7 @@
         <v>141</v>
       </c>
       <c r="C103" s="14">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>1004</v>
       </c>
       <c r="G103" s="14" t="s">
@@ -4985,11 +4985,11 @@
         <v>11</v>
       </c>
       <c r="R103" s="14" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S103" s="14" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>rm_optout_p1</v>
       </c>
       <c r="W103" s="14" t="s">
@@ -5010,7 +5010,7 @@
         <v>141</v>
       </c>
       <c r="C104" s="14">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>1005</v>
       </c>
       <c r="D104" s="14" t="s">
@@ -5031,11 +5031,11 @@
         <v>11</v>
       </c>
       <c r="R104" s="14" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S104" s="14" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>rm_optout_p1</v>
       </c>
       <c r="W104" s="14" t="s">
@@ -5056,7 +5056,7 @@
         <v>141</v>
       </c>
       <c r="C105" s="14">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>1006</v>
       </c>
       <c r="G105" s="14" t="s">
@@ -5074,11 +5074,11 @@
         <v>11</v>
       </c>
       <c r="R105" s="14" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S105" s="14" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>rm_optout_p1</v>
       </c>
       <c r="W105" s="5" t="str">
@@ -5105,7 +5105,7 @@
         <v>141</v>
       </c>
       <c r="C106" s="14">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>1007</v>
       </c>
       <c r="G106" s="14" t="s">
@@ -5123,11 +5123,11 @@
         <v>11</v>
       </c>
       <c r="R106" s="14" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S106" s="14" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>rm_optout_p1</v>
       </c>
       <c r="W106" s="14" t="s">
@@ -5151,7 +5151,7 @@
         <v>141</v>
       </c>
       <c r="C107" s="14">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>1008</v>
       </c>
       <c r="D107" s="14" t="s">
@@ -5172,11 +5172,11 @@
         <v>11</v>
       </c>
       <c r="R107" s="14" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S107" s="14" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>rm_optout_p1</v>
       </c>
       <c r="W107" s="14" t="s">
@@ -5200,7 +5200,7 @@
         <v>141</v>
       </c>
       <c r="C108" s="14">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>1009</v>
       </c>
       <c r="D108" s="14" t="s">
@@ -5221,11 +5221,11 @@
         <v>11</v>
       </c>
       <c r="R108" s="14" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S108" s="14" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>rm_optout_p1</v>
       </c>
       <c r="W108" s="14" t="s">
@@ -5246,7 +5246,7 @@
         <v>141</v>
       </c>
       <c r="C109" s="14">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>1010</v>
       </c>
       <c r="G109" s="14" t="s">
@@ -5264,11 +5264,11 @@
         <v>11</v>
       </c>
       <c r="R109" s="14" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S109" s="14" t="str">
-        <f t="shared" ref="S109" si="36">Q109</f>
+        <f t="shared" ref="S109" si="37">Q109</f>
         <v>rm_optout_p1</v>
       </c>
       <c r="W109" s="14" t="s">

</xml_diff>

<commit_message>
0.17.0: fixed issues with reqif_io QUERY_PASSWORD and selecting configuraiton
</commit_message>
<xml_diff>
--- a/elmclient/tests/tests_702.xlsx
+++ b/elmclient/tests/tests_702.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B073099B-4FDA-4E28-869F-2EDAC9172B2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7298B25-D64C-4012-AAEF-437E79F8894A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1414" yWindow="4080" windowWidth="24686" windowHeight="13054" xr2:uid="{E12FDD20-F1C7-4695-B929-60D3CA2A8B69}"/>
+    <workbookView xWindow="3077" yWindow="1346" windowWidth="29623" windowHeight="16105" xr2:uid="{E12FDD20-F1C7-4695-B929-60D3CA2A8B69}"/>
   </bookViews>
   <sheets>
     <sheet name="rmqueries" sheetId="1" r:id="rId1"/>
@@ -1162,7 +1162,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1172,9 +1172,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34CC5532-4E98-4C99-BC3C-1388DFEBC8F1}">
   <dimension ref="A1:AH111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F82" sqref="F82"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J82" sqref="J82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2651,7 +2651,7 @@
         <f t="shared" si="0"/>
         <v>tests\results\test131.csv</v>
       </c>
-      <c r="N34" s="5" t="s">
+      <c r="N34" s="6" t="s">
         <v>112</v>
       </c>
       <c r="Q34" s="5" t="s">
@@ -2694,7 +2694,7 @@
         <f t="shared" si="0"/>
         <v>tests\results\test132.csv</v>
       </c>
-      <c r="P35" s="5" t="s">
+      <c r="P35" s="6" t="s">
         <v>112</v>
       </c>
       <c r="Q35" s="5" t="s">
@@ -4432,7 +4432,7 @@
         <f t="shared" si="26"/>
         <v>tests\results\test312.csv</v>
       </c>
-      <c r="N82" s="4" t="s">
+      <c r="N82" s="11" t="s">
         <v>190</v>
       </c>
       <c r="Q82" s="4" t="s">

</xml_diff>